<commit_message>
update repo results with ned papers
</commit_message>
<xml_diff>
--- a/01 screening results.xlsx
+++ b/01 screening results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDA97B2-0D9B-4489-A25B-90140A8DA2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D139FB-4E9A-44C6-8A76-4E33181EA6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3660" uniqueCount="955">
   <si>
     <t>Reason for Exclusion</t>
   </si>
@@ -2882,12 +2882,84 @@
   <si>
     <t>Secondary study</t>
   </si>
+  <si>
+    <t>A Building Information Modeling (BIM)-Centric Digital Ecosystem for Smart Airport Life Cycle Management</t>
+  </si>
+  <si>
+    <t>Syracuse University ProQuest Dissertations &amp; Theses</t>
+  </si>
+  <si>
+    <t>Keskin, Basak</t>
+  </si>
+  <si>
+    <t>A Requirements Study on Model Repositories for Digital Twins in Construction Engineering</t>
+  </si>
+  <si>
+    <t>Cooperative Information Systems. CoopIS 2023</t>
+  </si>
+  <si>
+    <t>Zech, P., Fröch, G., Breu, R.</t>
+  </si>
+  <si>
+    <t>Applying Discrete Event Simulation on Patient Flow Scenarios with Health Monitoring Systems</t>
+  </si>
+  <si>
+    <t>Web Engineering. ICWE 2023</t>
+  </si>
+  <si>
+    <t>Gorelova, A., Meliá, S., Gadzhimusieva, D., Parichenko, A</t>
+  </si>
+  <si>
+    <t>Research on Digital Twin Technology of Small Hydraulic System</t>
+  </si>
+  <si>
+    <t>International Conference on Fluid Power and Mechatronics (FPM) </t>
+  </si>
+  <si>
+    <t>Wang, L., Li, B., Zhang, K., Wang, K., Huimin, H. A. O., &amp; Huang, J.</t>
+  </si>
+  <si>
+    <t>The hydraulic system is a common energy transmission and control system in the engineering field. It plays an important role in the fields of national economy and military industry, and has broad application prospects. The realization of intelligent operation and maintenance of hydraulic systems has become an important development direction in the industrial field. This study takes the small hydraulic system built in the laboratory as the research object, aiming at the problems of low twin model accuracy and insufficient generalization ability in the process of applying digital twin technology to realize intelligent operation and maintenance of the hydraulic system, the Kalman filter algorithm is used to build a high-fidelity hydraulic system digital twin model driven by a combination of mechanism and data, and the theoretically derived value of the mechanism simulation model is corrected through the data-driven results, and the Kalman filter algorithm is improved to make the twin model have higher accuracy and generalization ability. Finally, the twin model, expert system and visual interface are integrated to build an intelligent operation and maintenance platform for small hydraulic systems, which solves the technical problems of real-time evaluation of hydraulic system status and intelligent fault diagnosis, etc. and lays a foundation for the engineering of intelligent operation and maintenance mode of hydraulic system.</t>
+  </si>
+  <si>
+    <t>Despite technological advances, today there are still many treatments that have not been addressed by remote monitoring due to the absence of reliable monitoring devices and/or Health Monitoring Systems (HMS). In addition, there are situations where the deficiency of data due to the lack of a real scenario or device makes it impossible to use artificial intelligence (AI) techniques. However, this problem could be solved with simulation, being a fundamental mechanism for predicting and forecasting not-existing scenarios. In this paper, we proposed the use of Discrete-Event Simulation (DES) to model complex HMS scenarios. We have integrated a simulation module based on Matlab Simulink, into the MoSTHealth framework, so that the digital twins (DTs) modelled by the framework are elements of the DES scenario that the medical expert can easily parameterize through a mobile interface. A case study has been defined on the use of a wearable device (under development) that collects relevant hormone levels in real time, during infertility treatment. The DES simulation demonstrates an increase in the number of patients seen by one physician by 88,8%. In addition, the average waiting time for consultation decreased by 36.5%.</t>
+  </si>
+  <si>
+    <r>
+      <t>Building information modeling is becoming the preferred tool-assisted methodology in civil and construction engineering for the design, management, and creation of digital replicas of buildings. However, current tool support for creating and managing these </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>twins</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> is limited as of lacking interoperability at the model level. Yet, the Industry foundation classes describe a standardized format for exchanging models and data of buildings and bears a strong resemblance to the class- and object-based nature of the Unified modeling language. From this resemblance, we postulate the application of model-driven engineering for establishing a model repository as an open collaboration platform in Building information modeling. Based on our experience from ongoing and concluded interdisciplinary research projects in civil and construction engineering and computer science, in this paper, we seminally elicit requirements for such a model repository.</t>
+    </r>
+  </si>
+  <si>
+    <t>An increasing number of new airport infrastructure construction and improvement projects are being delivered in today’s modern world. However, value creation is a recurring issue due to inefficiencies in managing capital expenditures (CapEx) and operating expenses (OpEx), while trying to optimize project constraints of scope, time, cost, quality, and resources. In this new era of smart infrastructure, digitalization transforms the way projects are planned and delivered. Building Information Modeling (BIM) is a key digital process technique that has become an imperative for today’s Architecture, Engineering, Construction and Operations (AECO) sector. This research suggests a BIM-centric digital ecosystem by detailing technical and strategic aspects of Airport BIM implementation and digital technology integration from a life cycle perspective. This research provides a novel approach for consistent and continuous use of digital information between business and functional levels of an airport by developing a digital platform solution that will enable seamless flow of information across functions. Accordingly, this study targets to achieve three objectives: 1- To provide a scalable know-how of BIM-enabled digital transformation; 2- To guide airport owners and major stakeholders towards converging information siloes for airport life cycle data management by an Airport BIM Framework; 3- To develop a BIM-based digital platform architecture towards realization of an airport digital twin for airport infrastructure life cycle management. Airport infrastructures can be considered as a System of Systems (SoS). As such, Model Based Systems Engineering (MBSE) with Systems Modeling Language (SysML) is selected as the key methodology towards designing a digital ecosystem. Applying MBSE principles leads to forming an integrating framework for managing the digital ecosystem. Furthermore, this research adopts convergent parallel mixed methods to collect and analyze multiple forms of data. Data collection tools include extensive literature and industry review; an online questionnaire; semi-structured interviews with airport owner parties; focus group discussions; first-hand observations; and document reviews. Data analysis stage includes multiple explanatory case study analyses, thematic analysis, project mapping, percent coverage analysis for coded themes to achieve Objective 1; thematic analysis, cluster analysis, framework analysis, and non-parametric statistical analysis for Objective 2; and qualitative content analysis, non-parametric statistical analysis to accomplish Objective 3. This research presents a novel roadmap toward facilitation of smart airports with alignment and integration of disruptive technologies with business and operational aspects of airports. Multiple comprehensive case study analyses on international large-hub airports and triangulation of organization-level and project-level results systematically generate scalable technical and strategic guidelines for BIM implementation. The proposed platform architecture will incentivize major stakeholders for value-creation, data sharing, and control throughout a project life cycle. Introducing scalability and minimizing complexity for end-users through a digital platform approach will lead to a more connected environment. Consequently, a digital ecosystem enables sophisticated interaction between people, places, and assets. Model-driven approach provides an effective strategy for enhanced decision-making that helps optimization of project resources and allows fast adaptation to emerging business and operational demands. Accordingly, airport sustainability measures -economic vitality, operational efficiency, natural resources, and social responsibility- will improve due to higher levels of efficiency in CapEx and OpEx. Changes in business models for large capital investments and introducing sustainability to supply chains are among the anticipated broader impacts of this study.</t>
+  </si>
+  <si>
+    <t>NOk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2984,6 +3056,38 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -3035,7 +3139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3082,6 +3186,16 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3325,8 +3439,8 @@
   </sheetPr>
   <dimension ref="A1:U923"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C186" sqref="C186:H186"/>
+    <sheetView tabSelected="1" topLeftCell="D182" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G188" sqref="G188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12432,77 +12546,166 @@
       <c r="P186"/>
       <c r="Q186"/>
     </row>
-    <row r="187" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A187" s="19"/>
-      <c r="B187" s="19"/>
-      <c r="C187" s="19"/>
-      <c r="D187" s="19"/>
-      <c r="E187" s="19"/>
-      <c r="F187" s="19"/>
-      <c r="H187" s="18"/>
-      <c r="I187" s="18"/>
-      <c r="J187" s="19"/>
-      <c r="K187" s="19"/>
-      <c r="L187" s="21"/>
-      <c r="M187" s="18"/>
-      <c r="N187" s="18"/>
-      <c r="O187" s="18"/>
-      <c r="P187" s="18"/>
-      <c r="Q187" s="18"/>
-    </row>
-    <row r="188" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A188" s="19"/>
-      <c r="B188" s="19"/>
-      <c r="C188" s="19"/>
-      <c r="D188" s="19"/>
-      <c r="E188" s="19"/>
-      <c r="F188" s="19"/>
-      <c r="H188" s="18"/>
-      <c r="I188" s="18"/>
-      <c r="J188" s="19"/>
-      <c r="K188" s="19"/>
-      <c r="L188" s="21"/>
-      <c r="M188" s="18"/>
-      <c r="N188" s="18"/>
-      <c r="O188" s="18"/>
-      <c r="P188" s="18"/>
-      <c r="Q188" s="18"/>
-    </row>
-    <row r="189" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A189" s="19"/>
-      <c r="B189" s="19"/>
-      <c r="C189" s="19"/>
-      <c r="D189" s="19"/>
-      <c r="E189" s="19"/>
-      <c r="F189" s="19"/>
-      <c r="H189" s="18"/>
-      <c r="I189" s="18"/>
-      <c r="J189" s="19"/>
-      <c r="K189" s="19"/>
-      <c r="L189" s="21"/>
-      <c r="M189" s="18"/>
-      <c r="N189" s="18"/>
-      <c r="O189" s="18"/>
-      <c r="P189" s="18"/>
-      <c r="Q189" s="18"/>
-    </row>
-    <row r="190" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A190" s="19"/>
-      <c r="B190" s="19"/>
-      <c r="C190" s="19"/>
-      <c r="D190" s="19"/>
-      <c r="E190" s="19"/>
-      <c r="F190" s="19"/>
-      <c r="H190" s="18"/>
-      <c r="I190" s="18"/>
-      <c r="J190" s="19"/>
-      <c r="K190" s="19"/>
-      <c r="L190" s="21"/>
-      <c r="M190" s="18"/>
-      <c r="N190" s="18"/>
-      <c r="O190" s="18"/>
-      <c r="P190" s="18"/>
-      <c r="Q190" s="18"/>
+    <row r="187" spans="1:17" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>938</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>930</v>
+      </c>
+      <c r="D187" s="6" t="s">
+        <v>934</v>
+      </c>
+      <c r="E187" s="6" t="s">
+        <v>934</v>
+      </c>
+      <c r="F187" s="19" t="s">
+        <v>934</v>
+      </c>
+      <c r="G187" s="22" t="s">
+        <v>954</v>
+      </c>
+      <c r="L187" s="33" t="s">
+        <v>953</v>
+      </c>
+      <c r="M187" s="29" t="s">
+        <v>939</v>
+      </c>
+      <c r="N187" t="s">
+        <v>940</v>
+      </c>
+      <c r="O187">
+        <v>2021</v>
+      </c>
+      <c r="P187" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q187" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A188" s="30" t="s">
+        <v>941</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="C188" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="D188" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="E188" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="F188" s="34" t="s">
+        <v>930</v>
+      </c>
+      <c r="G188" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="L188" s="32" t="s">
+        <v>952</v>
+      </c>
+      <c r="M188" s="30" t="s">
+        <v>942</v>
+      </c>
+      <c r="N188" s="30" t="s">
+        <v>943</v>
+      </c>
+      <c r="O188">
+        <v>2023</v>
+      </c>
+      <c r="P188" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q188" s="30" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A189" s="30" t="s">
+        <v>944</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="D189" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="E189" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="F189" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="G189" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="L189" s="32" t="s">
+        <v>951</v>
+      </c>
+      <c r="M189" s="30" t="s">
+        <v>945</v>
+      </c>
+      <c r="N189" s="30" t="s">
+        <v>946</v>
+      </c>
+      <c r="O189">
+        <v>2023</v>
+      </c>
+      <c r="P189" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q189" s="30" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" ht="205.2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>947</v>
+      </c>
+      <c r="B190" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="C190" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="D190" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="E190" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="F190" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="G190" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="L190" s="31" t="s">
+        <v>950</v>
+      </c>
+      <c r="M190" t="s">
+        <v>948</v>
+      </c>
+      <c r="N190" t="s">
+        <v>949</v>
+      </c>
+      <c r="O190">
+        <v>2023</v>
+      </c>
+      <c r="Q190" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="191" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A191" s="19"/>
@@ -29857,10 +30060,10 @@
       <c r="A139" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="B139" s="29" t="s">
+      <c r="B139" s="35" t="s">
         <v>555</v>
       </c>
-      <c r="C139" s="30"/>
+      <c r="C139" s="36"/>
       <c r="D139" s="13" t="s">
         <v>500</v>
       </c>

</xml_diff>